<commit_message>
:up: algumas questões de cont de cust cadastradas e mais algumas respondidas
</commit_message>
<xml_diff>
--- a/banco_de_dados/historico_respostas.xlsx
+++ b/banco_de_dados/historico_respostas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
@@ -2599,6 +2599,544 @@
         <v>1</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:15</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>955</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Verbs</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:16</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>954</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Pronouns</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:16</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>953</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:37</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>952</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:38</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>951</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:40</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>980</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:41</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>979</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:43</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>978</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:44</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>977</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:47</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>976</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:47</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>975</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Pronouns</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:49</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>974</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:50</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>973</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:52</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>972</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:53</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>971</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:56</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>881</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:57</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>880</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>29/12/2025 21:58</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>879</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>29/12/2025 22:04</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>878</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Interpretação de Texto</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>29/12/2025 22:11</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>970</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Semantic</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>